<commit_message>
done with excel class
</commit_message>
<xml_diff>
--- a/Les Permis Excel.xlsx
+++ b/Les Permis Excel.xlsx
@@ -14,18 +14,213 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+  <x:si>
+    <x:t>numeroPermis</x:t>
+  </x:si>
   <x:si>
     <x:t>numeroDemmande</x:t>
   </x:si>
   <x:si>
-    <x:t>nomTitulaire</x:t>
-  </x:si>
-  <x:si>
-    <x:t>123</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Boutissante</x:t>
+    <x:t>dateDepotDemmande</x:t>
+  </x:si>
+  <x:si>
+    <x:t>type</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ex_permis</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Superficie</x:t>
+  </x:si>
+  <x:si>
+    <x:t>pointPivot</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Abscisse</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ordonne</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zone</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RaisonSocial</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Titulaire</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Region</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Province</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CodeProvince</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Commune</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Caidat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date_Institision</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Carte</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Echeance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NomSite</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DateDepart_CRI_CF_DMH_DR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DateReutor_CRI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date_Decision</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date_Enquete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Election_Domicile</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Effective</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Investisement_Realise</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Investisement_Projete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>occupation_temporaire</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Inscription_Conservation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3232</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-05-17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32343</x:t>
+  </x:si>
+  <x:si>
+    <x:t>point_pevot4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23423</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SARL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Societe2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Region1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Province4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1114</x:t>
+  </x:si>
+  <x:si>
+    <x:t>commune4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Caidat4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>carte4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>www.monsite.ma</x:t>
+  </x:si>
+  <x:si>
+    <x:t>234dgfasder</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>False</x:t>
+  </x:si>
+  <x:si>
+    <x:t>345</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-05-19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2342</x:t>
+  </x:si>
+  <x:si>
+    <x:t>point_pevot1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>34523</x:t>
+  </x:si>
+  <x:si>
+    <x:t>La Societe de Mazzouz</x:t>
+  </x:si>
+  <x:si>
+    <x:t>commune1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Caidat1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>carte2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>www.mazzouz.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mon Domicile</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>True</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-05-20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Le Plus Grand Societe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>carte1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Grant Societ</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -89,11 +284,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="LesPermis" displayName="LesPermis" ref="A1:B5" totalsRowShown="0">
-  <x:autoFilter ref="A1:B5"/>
-  <x:tableColumns count="2">
-    <x:tableColumn id="1" name="numeroDemmande"/>
-    <x:tableColumn id="2" name="nomTitulaire"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="LesPermis" displayName="LesPermis" ref="A1:AE5" totalsRowShown="0">
+  <x:autoFilter ref="A1:AE5"/>
+  <x:tableColumns count="31">
+    <x:tableColumn id="1" name="numeroPermis"/>
+    <x:tableColumn id="2" name="numeroDemmande"/>
+    <x:tableColumn id="3" name="dateDepotDemmande"/>
+    <x:tableColumn id="4" name="type"/>
+    <x:tableColumn id="5" name="ex_permis"/>
+    <x:tableColumn id="6" name="Superficie"/>
+    <x:tableColumn id="7" name="pointPivot"/>
+    <x:tableColumn id="8" name="Abscisse"/>
+    <x:tableColumn id="9" name="Ordonne"/>
+    <x:tableColumn id="10" name="Zone"/>
+    <x:tableColumn id="11" name="RaisonSocial"/>
+    <x:tableColumn id="12" name="Titulaire"/>
+    <x:tableColumn id="13" name="Region"/>
+    <x:tableColumn id="14" name="Province"/>
+    <x:tableColumn id="15" name="CodeProvince"/>
+    <x:tableColumn id="16" name="Commune"/>
+    <x:tableColumn id="17" name="Caidat"/>
+    <x:tableColumn id="18" name="Date_Institision"/>
+    <x:tableColumn id="19" name="Carte"/>
+    <x:tableColumn id="20" name="Echeance"/>
+    <x:tableColumn id="21" name="NomSite"/>
+    <x:tableColumn id="22" name="DateDepart_CRI_CF_DMH_DR"/>
+    <x:tableColumn id="23" name="DateReutor_CRI"/>
+    <x:tableColumn id="24" name="Date_Decision"/>
+    <x:tableColumn id="25" name="Date_Enquete"/>
+    <x:tableColumn id="26" name="Election_Domicile"/>
+    <x:tableColumn id="27" name="Effective"/>
+    <x:tableColumn id="28" name="Investisement_Realise"/>
+    <x:tableColumn id="29" name="Investisement_Projete"/>
+    <x:tableColumn id="30" name="occupation_temporaire"/>
+    <x:tableColumn id="31" name="Inscription_Conservation"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -387,50 +611,419 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B5"/>
+  <x:dimension ref="A1:AE5"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:2">
+    <x:row r="1" spans="1:31">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="L1" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="M1" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="N1" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="O1" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="P1" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="Q1" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="R1" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="S1" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="T1" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="U1" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="V1" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="W1" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="X1" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="Y1" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="Z1" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="AA1" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="AB1" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="AC1" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="AD1" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="AE1" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:2">
+    <x:row r="2" spans="1:31">
       <x:c r="A2" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K2" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="L2" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="M2" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N2" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O2" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P2" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="Q2" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="R2" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="S2" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="T2" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="U2" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="V2" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="W2" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="X2" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Y2" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Z2" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AA2" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="AB2" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC2" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AD2" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AE2" s="0" t="s">
+        <x:v>51</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:2">
+    <x:row r="3" spans="1:31">
       <x:c r="A3" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K3" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="L3" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="M3" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N3" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O3" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P3" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q3" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R3" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="S3" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="T3" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="U3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="V3" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="W3" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="X3" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="Y3" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="Z3" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="AA3" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="AB3" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC3" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE3" s="0" t="s">
+        <x:v>64</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:2">
+    <x:row r="4" spans="1:31">
       <x:c r="A4" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="L4" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="M4" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N4" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O4" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P4" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q4" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R4" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="S4" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T4" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="V4" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="W4" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="X4" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="Y4" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="AB4" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC4" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE4" s="0" t="s">
+        <x:v>51</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:2">
+    <x:row r="5" spans="1:31">
       <x:c r="A5" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="L5" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="M5" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N5" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O5" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P5" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q5" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R5" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="S5" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T5" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="V5" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="W5" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="X5" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="Y5" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="AB5" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC5" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE5" s="0" t="s">
+        <x:v>51</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
i have updated the path of excel to dynamic path
</commit_message>
<xml_diff>
--- a/Les Permis Excel.xlsx
+++ b/Les Permis Excel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <x:si>
     <x:t>numeroPermis</x:t>
   </x:si>
@@ -221,6 +221,30 @@
   </x:si>
   <x:si>
     <x:t>Grant Societ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>77</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-05-30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>66</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sarl</x:t>
+  </x:si>
+  <x:si>
+    <x:t>88</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-05-31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fsdf</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -284,8 +308,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="LesPermis" displayName="LesPermis" ref="A1:AE5" totalsRowShown="0">
-  <x:autoFilter ref="A1:AE5"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="LesPermis" displayName="LesPermis" ref="A1:AE33" totalsRowShown="0">
+  <x:autoFilter ref="A1:AE33"/>
   <x:tableColumns count="31">
     <x:tableColumn id="1" name="numeroPermis"/>
     <x:tableColumn id="2" name="numeroDemmande"/>
@@ -611,7 +635,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:AE5"/>
+  <x:dimension ref="A1:AE33"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1023,6 +1047,1835 @@
         <x:v>49</x:v>
       </x:c>
       <x:c r="AE5" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:31">
+      <x:c r="A6" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M6" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N6" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O6" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P6" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q6" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R6" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S6" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T6" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V6" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W6" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X6" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y6" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB6" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC6" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE6" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:31">
+      <x:c r="A7" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M7" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N7" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O7" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P7" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q7" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R7" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S7" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T7" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V7" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W7" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X7" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y7" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB7" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC7" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE7" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:31">
+      <x:c r="A8" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M8" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N8" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O8" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P8" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q8" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R8" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S8" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T8" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V8" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W8" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X8" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y8" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB8" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC8" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE8" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:31">
+      <x:c r="A9" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M9" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N9" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O9" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P9" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q9" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R9" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S9" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T9" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V9" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W9" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X9" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y9" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB9" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC9" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE9" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:31">
+      <x:c r="A10" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M10" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N10" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O10" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P10" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q10" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R10" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S10" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T10" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V10" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W10" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X10" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y10" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB10" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC10" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE10" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:31">
+      <x:c r="A11" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G11" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M11" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N11" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O11" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P11" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q11" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R11" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S11" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T11" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V11" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W11" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X11" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y11" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB11" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC11" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE11" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:31">
+      <x:c r="A12" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M12" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N12" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O12" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P12" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q12" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R12" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S12" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T12" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V12" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W12" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X12" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y12" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB12" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC12" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE12" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:31">
+      <x:c r="A13" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G13" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M13" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N13" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O13" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P13" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q13" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R13" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S13" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T13" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V13" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W13" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X13" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y13" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB13" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC13" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE13" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:31">
+      <x:c r="A14" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G14" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M14" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N14" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O14" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P14" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q14" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R14" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S14" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T14" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V14" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W14" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X14" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y14" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB14" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC14" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE14" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:31">
+      <x:c r="A15" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G15" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M15" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N15" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O15" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P15" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q15" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R15" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S15" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T15" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V15" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W15" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X15" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y15" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB15" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC15" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE15" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:31">
+      <x:c r="A16" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G16" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M16" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N16" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O16" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P16" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q16" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R16" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S16" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T16" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V16" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W16" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X16" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y16" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB16" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC16" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE16" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:31">
+      <x:c r="A17" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G17" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M17" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N17" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O17" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P17" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q17" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R17" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S17" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T17" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V17" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W17" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X17" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y17" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB17" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC17" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE17" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:31">
+      <x:c r="A18" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G18" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M18" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N18" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O18" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P18" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q18" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R18" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S18" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T18" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V18" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W18" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X18" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y18" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB18" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC18" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE18" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:31">
+      <x:c r="A19" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G19" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M19" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N19" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O19" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P19" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q19" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R19" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S19" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T19" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V19" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W19" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X19" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y19" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB19" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC19" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE19" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:31">
+      <x:c r="A20" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G20" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M20" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N20" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O20" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P20" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q20" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R20" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S20" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T20" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V20" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W20" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X20" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y20" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB20" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC20" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE20" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:31">
+      <x:c r="A21" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G21" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M21" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N21" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O21" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P21" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q21" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R21" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S21" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T21" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V21" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W21" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X21" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y21" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB21" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC21" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE21" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:31">
+      <x:c r="A22" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G22" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M22" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N22" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O22" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P22" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q22" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R22" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S22" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T22" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V22" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W22" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X22" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y22" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB22" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC22" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE22" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:31">
+      <x:c r="A23" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F23" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G23" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M23" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N23" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O23" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P23" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q23" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R23" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S23" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T23" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V23" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W23" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X23" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y23" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB23" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC23" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE23" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:31">
+      <x:c r="A24" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F24" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G24" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M24" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N24" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O24" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P24" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q24" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R24" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S24" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T24" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V24" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W24" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X24" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y24" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB24" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC24" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE24" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:31">
+      <x:c r="A25" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G25" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M25" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N25" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O25" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P25" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q25" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R25" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S25" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T25" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V25" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W25" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X25" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y25" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB25" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC25" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE25" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:31">
+      <x:c r="A26" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F26" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G26" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M26" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N26" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O26" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P26" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q26" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R26" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S26" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T26" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V26" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W26" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X26" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y26" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB26" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC26" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE26" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:31">
+      <x:c r="A27" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G27" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M27" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N27" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O27" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P27" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q27" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R27" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S27" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T27" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V27" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W27" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X27" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y27" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB27" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC27" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE27" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:31">
+      <x:c r="A28" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G28" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M28" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N28" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O28" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P28" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q28" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R28" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S28" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T28" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V28" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W28" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X28" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y28" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB28" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC28" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE28" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:31">
+      <x:c r="A29" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G29" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M29" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N29" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O29" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P29" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q29" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R29" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S29" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T29" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V29" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W29" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X29" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y29" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB29" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC29" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE29" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:31">
+      <x:c r="A30" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F30" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G30" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M30" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N30" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O30" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P30" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q30" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R30" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S30" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T30" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V30" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W30" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X30" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y30" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB30" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC30" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE30" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:31">
+      <x:c r="A31" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F31" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G31" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="K31" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="M31" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N31" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O31" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P31" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q31" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R31" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S31" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T31" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V31" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W31" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X31" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y31" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB31" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC31" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE31" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:31">
+      <x:c r="A32" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F32" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G32" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="M32" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N32" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O32" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P32" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q32" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R32" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="S32" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T32" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="V32" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W32" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="X32" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Y32" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AB32" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC32" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE32" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:31">
+      <x:c r="A33" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F33" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G33" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="L33" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="M33" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N33" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O33" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P33" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Q33" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="R33" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="S33" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="T33" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="V33" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="W33" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="X33" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Y33" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Z33" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="AB33" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AC33" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE33" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
     </x:row>

</xml_diff>